<commit_message>
excel vba set up
</commit_message>
<xml_diff>
--- a/DataSheet/Data_Resources.xlsx
+++ b/DataSheet/Data_Resources.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\Unity 2D\GreatGame\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BCD648-2C58-4CBB-8C1A-FED0BD07BE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97746463-32FE-4D32-B9FB-678E45431062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30990" yWindow="2130" windowWidth="21600" windowHeight="11385" xr2:uid="{A8CE4FC6-529A-4D28-B9E0-C345F306D5DC}"/>
+    <workbookView xWindow="2940" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{A8CE4FC6-529A-4D28-B9E0-C345F306D5DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,27 +38,27 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>[CommonConfig]</t>
+    <t>CommonConfig</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#memo</t>
+    <t>FileName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Value</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Index</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>INITIAL_SUPPLY_AMOUNT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>INITIAL_MONEY_AMOUNT</t>
+    <t>INITIAL_MONEY_VALUE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INITIAL_SUPPLY_VALUE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -66,7 +66,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,7 +92,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="0"/>
       <name val="맑은 고딕"/>
@@ -101,7 +108,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
@@ -110,15 +116,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,14 +156,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79995117038483843"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -173,24 +190,42 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -207,6 +242,84 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>1343025</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>609600</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Button 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="54864" tIns="59436" rIns="54864" bIns="59436" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="ko-KR" altLang="en-US" sz="2200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="맑은 고딕"/>
+                  <a:ea typeface="맑은 고딕"/>
+                </a:rPr>
+                <a:t>Export</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -525,8 +638,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9055F364-34CC-4C53-AA40-00CA18C69C70}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9055F364-34CC-4C53-AA40-00CA18C69C70}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -534,44 +648,92 @@
   <cols>
     <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
+        <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5">
-        <v>50</v>
+      <c r="C10" s="1">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1025" r:id="rId3" name="Button 1">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!Jsonconverter">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>1343025</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>609600</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>